<commit_message>
[MOSIP-14369] Field values corrected
</commit_message>
<xml_diff>
--- a/deployment/v3/mosip/kernel/masterdata/upload/xlsx/app_authentication_method.xlsx
+++ b/deployment/v3/mosip/kernel/masterdata/upload/xlsx/app_authentication_method.xlsx
@@ -195,8 +195,8 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -218,14 +218,14 @@
   </sheetPr>
   <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.48"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.48"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -247,27 +247,27 @@
       <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="0" t="s">
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="n">
@@ -276,22 +276,22 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="0" t="s">
+      <c r="D3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G3" s="2" t="n">
@@ -300,22 +300,22 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="0" t="s">
+      <c r="D4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G4" s="2" t="n">
@@ -324,22 +324,22 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="0" t="s">
+      <c r="D5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G5" s="2" t="n">
@@ -348,22 +348,22 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="0" t="s">
+      <c r="D6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G6" s="2" t="n">
@@ -372,22 +372,22 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="0" t="s">
+      <c r="D7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="n">
@@ -396,22 +396,22 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="0" t="s">
+      <c r="D8" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G8" s="2" t="n">
@@ -420,22 +420,22 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="D9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G9" s="2" t="n">
@@ -444,22 +444,22 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="0" t="s">
+      <c r="D10" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="F10" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G10" s="2" t="n">
@@ -468,22 +468,22 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="D11" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="0" t="n">
+      <c r="F11" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G11" s="2" t="n">
@@ -492,22 +492,22 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G12" s="2" t="n">
@@ -516,22 +516,22 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="D13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G13" s="2" t="n">
@@ -540,22 +540,22 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="D14" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G14" s="2" t="n">
@@ -564,22 +564,22 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="D15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G15" s="2" t="n">
@@ -588,22 +588,22 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="D16" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G16" s="2" t="n">
@@ -612,22 +612,22 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
+      <c r="A17" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="0" t="s">
+      <c r="D17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="F17" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G17" s="2" t="n">
@@ -636,22 +636,22 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
+      <c r="A18" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="0" t="s">
+      <c r="D18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="0" t="n">
+      <c r="F18" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G18" s="2" t="n">
@@ -660,22 +660,22 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
+      <c r="A19" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="0" t="s">
+      <c r="D19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="0" t="n">
+      <c r="F19" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G19" s="2" t="n">
@@ -684,22 +684,22 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
+      <c r="A20" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="0" t="s">
+      <c r="D20" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="0" t="n">
+      <c r="F20" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G20" s="2" t="n">
@@ -708,22 +708,22 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
+      <c r="A21" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="0" t="s">
+      <c r="D21" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="0" t="n">
+      <c r="F21" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G21" s="2" t="n">
@@ -732,22 +732,22 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
+      <c r="A22" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="0" t="s">
+      <c r="D22" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="0" t="n">
+      <c r="F22" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G22" s="2" t="n">
@@ -756,22 +756,22 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
+      <c r="A23" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="0" t="s">
+      <c r="D23" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="0" t="n">
+      <c r="F23" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G23" s="2" t="n">
@@ -780,22 +780,22 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
+      <c r="A24" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="0" t="s">
+      <c r="D24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="0" t="n">
+      <c r="F24" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G24" s="2" t="n">
@@ -804,22 +804,22 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
+      <c r="A25" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="0" t="s">
+      <c r="D25" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="0" t="n">
+      <c r="F25" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G25" s="2" t="n">
@@ -828,22 +828,22 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
+      <c r="A26" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="0" t="s">
+      <c r="D26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="0" t="n">
+      <c r="F26" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G26" s="2" t="n">
@@ -852,22 +852,22 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
+      <c r="A27" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="0" t="s">
+      <c r="D27" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="0" t="n">
+      <c r="F27" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G27" s="2" t="n">
@@ -876,22 +876,22 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="A28" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="0" t="s">
+      <c r="D28" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="0" t="n">
+      <c r="F28" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G28" s="2" t="n">
@@ -900,22 +900,22 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
+      <c r="A29" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="0" t="s">
+      <c r="D29" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="0" t="n">
+      <c r="F29" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G29" s="2" t="n">
@@ -924,22 +924,22 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
+      <c r="A30" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="D30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="0" t="n">
+      <c r="F30" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G30" s="2" t="n">
@@ -948,22 +948,22 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
+      <c r="A31" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="0" t="s">
+      <c r="D31" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="0" t="n">
+      <c r="F31" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G31" s="2" t="n">
@@ -972,22 +972,22 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
+      <c r="A32" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="0" t="s">
+      <c r="D32" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="0" t="n">
+      <c r="F32" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G32" s="2" t="n">
@@ -996,22 +996,22 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+      <c r="A33" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="0" t="s">
+      <c r="D33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="0" t="n">
+      <c r="F33" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G33" s="2" t="n">
@@ -1020,22 +1020,22 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+      <c r="A34" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="0" t="s">
+      <c r="D34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="0" t="n">
+      <c r="F34" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G34" s="2" t="n">
@@ -1044,22 +1044,22 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
+      <c r="A35" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="0" t="s">
+      <c r="D35" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="0" t="n">
+      <c r="F35" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G35" s="2" t="n">
@@ -1068,22 +1068,22 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
+      <c r="A36" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="0" t="s">
+      <c r="D36" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="0" t="n">
+      <c r="F36" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G36" s="2" t="n">
@@ -1092,22 +1092,22 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
+      <c r="A37" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="0" t="s">
+      <c r="D37" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="0" t="n">
+      <c r="F37" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G37" s="2" t="n">
@@ -1116,22 +1116,22 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="0" t="s">
+      <c r="A38" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C38" s="0" t="s">
+      <c r="C38" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="0" t="s">
+      <c r="D38" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="0" t="n">
+      <c r="F38" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G38" s="2" t="n">
@@ -1140,22 +1140,22 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="s">
+      <c r="A39" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C39" s="0" t="s">
+      <c r="C39" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="0" t="s">
+      <c r="D39" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="0" t="n">
+      <c r="F39" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G39" s="2" t="n">
@@ -1164,22 +1164,22 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
+      <c r="A40" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C40" s="0" t="s">
+      <c r="C40" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="0" t="s">
+      <c r="D40" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="0" t="n">
+      <c r="F40" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G40" s="2" t="n">
@@ -1188,22 +1188,22 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="s">
+      <c r="A41" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C41" s="0" t="s">
+      <c r="C41" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="0" t="s">
+      <c r="D41" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F41" s="0" t="n">
+      <c r="F41" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G41" s="2" t="n">
@@ -1212,22 +1212,22 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0" t="s">
+      <c r="A42" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C42" s="0" t="s">
+      <c r="C42" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="0" t="s">
+      <c r="D42" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="0" t="n">
+      <c r="F42" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G42" s="2" t="n">
@@ -1236,22 +1236,22 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="s">
+      <c r="A43" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C43" s="0" t="s">
+      <c r="C43" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D43" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="0" t="s">
+      <c r="D43" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F43" s="0" t="n">
+      <c r="F43" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G43" s="2" t="n">
@@ -1260,22 +1260,22 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="s">
+      <c r="A44" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C44" s="0" t="s">
+      <c r="C44" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="0" t="s">
+      <c r="D44" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="0" t="n">
+      <c r="F44" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G44" s="2" t="n">
@@ -1284,22 +1284,22 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="s">
+      <c r="A45" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C45" s="0" t="s">
+      <c r="C45" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="0" t="s">
+      <c r="D45" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="0" t="n">
+      <c r="F45" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G45" s="2" t="n">
@@ -1308,22 +1308,22 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
+      <c r="A46" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C46" s="0" t="s">
+      <c r="C46" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D46" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" s="0" t="s">
+      <c r="D46" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="0" t="n">
+      <c r="F46" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G46" s="2" t="n">
@@ -1332,22 +1332,22 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="0" t="s">
+      <c r="A47" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C47" s="0" t="s">
+      <c r="C47" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="0" t="s">
+      <c r="D47" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F47" s="0" t="n">
+      <c r="F47" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G47" s="2" t="n">
@@ -1356,22 +1356,22 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="s">
+      <c r="A48" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C48" s="0" t="s">
+      <c r="C48" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E48" s="0" t="s">
+      <c r="D48" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F48" s="0" t="n">
+      <c r="F48" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G48" s="2" t="n">
@@ -1380,22 +1380,22 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="s">
+      <c r="A49" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C49" s="0" t="s">
+      <c r="C49" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" s="0" t="s">
+      <c r="D49" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F49" s="0" t="n">
+      <c r="F49" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G49" s="2" t="n">
@@ -1404,22 +1404,22 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="s">
+      <c r="A50" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="C50" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="0" t="s">
+      <c r="D50" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="0" t="n">
+      <c r="F50" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G50" s="2" t="n">
@@ -1428,22 +1428,22 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0" t="s">
+      <c r="A51" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C51" s="0" t="s">
+      <c r="C51" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="0" t="s">
+      <c r="D51" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F51" s="0" t="n">
+      <c r="F51" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G51" s="2" t="n">
@@ -1452,22 +1452,22 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
+      <c r="A52" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B52" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C52" s="0" t="s">
+      <c r="C52" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D52" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" s="0" t="s">
+      <c r="D52" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F52" s="0" t="n">
+      <c r="F52" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G52" s="2" t="n">
@@ -1476,22 +1476,22 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="s">
+      <c r="A53" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B53" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C53" s="0" t="s">
+      <c r="C53" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D53" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="0" t="s">
+      <c r="D53" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F53" s="0" t="n">
+      <c r="F53" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G53" s="2" t="n">
@@ -1500,22 +1500,22 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="s">
+      <c r="A54" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B54" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C54" s="0" t="s">
+      <c r="C54" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D54" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="0" t="s">
+      <c r="D54" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="0" t="n">
+      <c r="F54" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G54" s="2" t="n">
@@ -1524,22 +1524,22 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="0" t="s">
+      <c r="A55" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B55" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C55" s="0" t="s">
+      <c r="C55" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D55" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="0" t="s">
+      <c r="D55" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F55" s="0" t="n">
+      <c r="F55" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G55" s="2" t="n">
@@ -1548,22 +1548,22 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="s">
+      <c r="A56" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B56" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C56" s="0" t="s">
+      <c r="C56" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="0" t="s">
+      <c r="D56" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F56" s="0" t="n">
+      <c r="F56" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G56" s="2" t="n">
@@ -1572,22 +1572,22 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="s">
+      <c r="A57" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B57" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C57" s="0" t="s">
+      <c r="C57" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="0" t="s">
+      <c r="D57" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="0" t="n">
+      <c r="F57" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G57" s="2" t="n">
@@ -1596,22 +1596,22 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
+      <c r="A58" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B58" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C58" s="0" t="s">
+      <c r="C58" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E58" s="0" t="s">
+      <c r="D58" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F58" s="0" t="n">
+      <c r="F58" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G58" s="2" t="n">
@@ -1620,22 +1620,22 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="0" t="s">
+      <c r="A59" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B59" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C59" s="0" t="s">
+      <c r="C59" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D59" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E59" s="0" t="s">
+      <c r="D59" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="0" t="n">
+      <c r="F59" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G59" s="2" t="n">
@@ -1644,22 +1644,22 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="0" t="s">
+      <c r="A60" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B60" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C60" s="0" t="s">
+      <c r="C60" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D60" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E60" s="0" t="s">
+      <c r="D60" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="0" t="n">
+      <c r="F60" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G60" s="2" t="n">
@@ -1668,22 +1668,22 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="s">
+      <c r="A61" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C61" s="0" t="s">
+      <c r="C61" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E61" s="0" t="s">
+      <c r="D61" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F61" s="0" t="n">
+      <c r="F61" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G61" s="2" t="n">
@@ -1692,22 +1692,22 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="s">
+      <c r="A62" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C62" s="0" t="s">
+      <c r="C62" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E62" s="0" t="s">
+      <c r="D62" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F62" s="0" t="n">
+      <c r="F62" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G62" s="2" t="n">
@@ -1716,22 +1716,22 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="s">
+      <c r="A63" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B63" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C63" s="0" t="s">
+      <c r="C63" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E63" s="0" t="s">
+      <c r="D63" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="0" t="n">
+      <c r="F63" s="5" t="n">
         <v>1</v>
       </c>
       <c r="G63" s="2" t="n">
@@ -1740,22 +1740,22 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="s">
+      <c r="A64" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B64" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C64" s="0" t="s">
+      <c r="C64" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D64" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E64" s="0" t="s">
+      <c r="D64" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F64" s="0" t="n">
+      <c r="F64" s="5" t="n">
         <v>2</v>
       </c>
       <c r="G64" s="2" t="n">
@@ -1764,22 +1764,22 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="0" t="s">
+      <c r="A65" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B65" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C65" s="0" t="s">
+      <c r="C65" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D65" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E65" s="0" t="s">
+      <c r="D65" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F65" s="0" t="n">
+      <c r="F65" s="5" t="n">
         <v>3</v>
       </c>
       <c r="G65" s="2" t="n">
@@ -1788,22 +1788,22 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="0" t="s">
+      <c r="A66" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B66" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C66" s="0" t="s">
+      <c r="C66" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D66" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E66" s="0" t="s">
+      <c r="D66" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F66" s="0" t="n">
+      <c r="F66" s="5" t="n">
         <v>4</v>
       </c>
       <c r="G66" s="2" t="n">
@@ -1812,22 +1812,22 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="0" t="s">
+      <c r="A67" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C67" s="0" t="s">
+      <c r="C67" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E67" s="0" t="s">
+      <c r="D67" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F67" s="0" t="n">
+      <c r="F67" s="5" t="n">
         <v>5</v>
       </c>
       <c r="G67" s="2" t="n">
@@ -1838,7 +1838,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
[MOSIP-14369] Fix: boolean field values
</commit_message>
<xml_diff>
--- a/deployment/v3/mosip/kernel/masterdata/upload/xlsx/app_authentication_method.xlsx
+++ b/deployment/v3/mosip/kernel/masterdata/upload/xlsx/app_authentication_method.xlsx
@@ -89,10 +89,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
-    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -174,16 +173,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -219,1618 +214,1618 @@
   <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J13" activeCellId="0" sqref="J13"/>
+      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.49"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="8.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.49"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="5" t="s">
+      <c r="D2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G2" s="2" t="n">
+      <c r="F2" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5" t="n">
+      <c r="F3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="5" t="n">
+      <c r="F4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="D5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="5" t="n">
+      <c r="F5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="5" t="s">
+      <c r="D6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="5" t="n">
+      <c r="F6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" s="5" t="s">
+      <c r="D7" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2" t="n">
+      <c r="F7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="5" t="s">
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="5" t="n">
+      <c r="F8" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="5" t="n">
+      <c r="F9" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E10" s="5" t="s">
+      <c r="D10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F10" s="5" t="n">
+      <c r="F10" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="5" t="s">
+      <c r="D11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="5" t="n">
+      <c r="F11" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="5" t="s">
+      <c r="D12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2" t="n">
+      <c r="F12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="5" t="n">
+      <c r="F13" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B14" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C14" s="5" t="s">
+      <c r="C14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="5" t="s">
+      <c r="D14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="5" t="n">
+      <c r="F14" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B15" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="5" t="s">
+      <c r="D15" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="5" t="n">
+      <c r="F15" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="D16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="5" t="n">
+      <c r="F16" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="5" t="s">
+      <c r="D17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2" t="n">
+      <c r="F17" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B18" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="5" t="s">
+      <c r="D18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="5" t="n">
+      <c r="F18" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G18" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B19" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D19" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="5" t="s">
+      <c r="D19" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G19" s="2" t="n">
+      <c r="F19" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B20" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" s="5" t="s">
+      <c r="D20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="5" t="n">
+      <c r="F20" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G20" s="2" t="n">
+      <c r="G20" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E21" s="5" t="s">
+      <c r="D21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F21" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G21" s="2" t="n">
+      <c r="F21" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B22" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E22" s="5" t="s">
+      <c r="D22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="5" t="n">
+      <c r="F22" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G22" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="C23" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="5" t="s">
+      <c r="D23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F23" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G23" s="2" t="n">
+      <c r="F23" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B24" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E24" s="5" t="s">
+      <c r="D24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="5" t="n">
+      <c r="F24" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G24" s="2" t="n">
+      <c r="G24" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B25" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="5" t="s">
+      <c r="D25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="5" t="n">
+      <c r="F25" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G25" s="2" t="n">
+      <c r="G25" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E26" s="5" t="s">
+      <c r="D26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="5" t="n">
+      <c r="F26" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G26" s="2" t="n">
+      <c r="G26" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B27" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E27" s="5" t="s">
+      <c r="D27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F27" s="5" t="n">
+      <c r="F27" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="G27" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B28" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="5" t="s">
+      <c r="D28" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G28" s="2" t="n">
+      <c r="F28" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B29" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="5" t="s">
+      <c r="D29" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="5" t="n">
+      <c r="F29" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G29" s="2" t="n">
+      <c r="G29" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="5" t="s">
+      <c r="D30" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F30" s="5" t="n">
+      <c r="F30" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G30" s="2" t="n">
+      <c r="G30" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="5" t="s">
+      <c r="A31" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="5" t="s">
+      <c r="D31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="5" t="n">
+      <c r="F31" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G31" s="2" t="n">
+      <c r="G31" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="5" t="s">
+      <c r="D32" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F32" s="5" t="n">
+      <c r="F32" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G32" s="2" t="n">
+      <c r="G32" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B33" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E33" s="5" t="s">
+      <c r="D33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F33" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G33" s="2" t="n">
+      <c r="F33" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G33" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B34" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="5" t="s">
+      <c r="D34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="5" t="n">
+      <c r="F34" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G34" s="2" t="n">
+      <c r="G34" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E35" s="5" t="s">
+      <c r="D35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E35" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F35" s="5" t="n">
+      <c r="F35" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G35" s="2" t="n">
+      <c r="G35" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B36" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C36" s="5" t="s">
+      <c r="C36" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E36" s="5" t="s">
+      <c r="D36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="5" t="n">
+      <c r="F36" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G36" s="2" t="n">
+      <c r="G36" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C37" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E37" s="5" t="s">
+      <c r="D37" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E37" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F37" s="5" t="n">
+      <c r="F37" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G37" s="2" t="n">
+      <c r="G37" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C38" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E38" s="5" t="s">
+      <c r="D38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E38" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F38" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G38" s="2" t="n">
+      <c r="F38" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C39" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E39" s="5" t="s">
+      <c r="D39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E39" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F39" s="5" t="n">
+      <c r="F39" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G39" s="2" t="n">
+      <c r="G39" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E40" s="5" t="s">
+      <c r="D40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="5" t="n">
+      <c r="F40" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G40" s="2" t="n">
+      <c r="G40" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E41" s="5" t="s">
+      <c r="D41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F41" s="5" t="n">
+      <c r="F41" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G41" s="2" t="n">
+      <c r="G41" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C42" s="5" t="s">
+      <c r="C42" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E42" s="5" t="s">
+      <c r="D42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F42" s="5" t="n">
+      <c r="F42" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G42" s="2" t="n">
+      <c r="G42" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C43" s="5" t="s">
+      <c r="C43" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="5" t="s">
+      <c r="D43" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F43" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G43" s="2" t="n">
+      <c r="F43" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G43" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="5" t="s">
+      <c r="D44" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F44" s="5" t="n">
+      <c r="F44" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G44" s="2" t="n">
+      <c r="G44" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B45" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D45" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="5" t="s">
+      <c r="D45" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F45" s="5" t="n">
+      <c r="F45" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G45" s="2" t="n">
+      <c r="G45" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B46" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C46" s="5" t="s">
+      <c r="C46" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" s="5" t="s">
+      <c r="D46" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F46" s="5" t="n">
+      <c r="F46" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G46" s="2" t="n">
+      <c r="G46" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C47" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="5" t="s">
+      <c r="D47" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F47" s="5" t="n">
+      <c r="F47" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G47" s="2" t="n">
+      <c r="G47" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5" t="s">
+      <c r="A48" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B48" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C48" s="5" t="s">
+      <c r="C48" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E48" s="5" t="s">
+      <c r="D48" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E48" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F48" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G48" s="2" t="n">
+      <c r="F48" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G48" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E49" s="5" t="s">
+      <c r="D49" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F49" s="5" t="n">
+      <c r="F49" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G49" s="2" t="n">
+      <c r="G49" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B50" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C50" s="5" t="s">
+      <c r="C50" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E50" s="5" t="s">
+      <c r="D50" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F50" s="5" t="n">
+      <c r="F50" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G50" s="2" t="n">
+      <c r="G50" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B51" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C51" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E51" s="5" t="s">
+      <c r="D51" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F51" s="5" t="n">
+      <c r="F51" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G51" s="2" t="n">
+      <c r="G51" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B52" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C52" s="5" t="s">
+      <c r="C52" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E52" s="5" t="s">
+      <c r="D52" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F52" s="5" t="n">
+      <c r="F52" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G52" s="2" t="n">
+      <c r="G52" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5" t="s">
+      <c r="A53" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B53" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E53" s="5" t="s">
+      <c r="D53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E53" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F53" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G53" s="2" t="n">
+      <c r="F53" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G53" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B54" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C54" s="5" t="s">
+      <c r="C54" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="5" t="s">
+      <c r="D54" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E54" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F54" s="5" t="n">
+      <c r="F54" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G54" s="2" t="n">
+      <c r="G54" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B55" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C55" s="5" t="s">
+      <c r="C55" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D55" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E55" s="5" t="s">
+      <c r="D55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E55" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F55" s="5" t="n">
+      <c r="F55" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G55" s="2" t="n">
+      <c r="G55" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B56" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C56" s="5" t="s">
+      <c r="C56" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D56" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E56" s="5" t="s">
+      <c r="D56" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E56" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F56" s="5" t="n">
+      <c r="F56" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G56" s="2" t="n">
+      <c r="G56" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B57" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C57" s="5" t="s">
+      <c r="C57" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D57" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E57" s="5" t="s">
+      <c r="D57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E57" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F57" s="5" t="n">
+      <c r="F57" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G57" s="2" t="n">
+      <c r="G57" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="5" t="s">
+      <c r="A58" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B58" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D58" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E58" s="5" t="s">
+      <c r="D58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E58" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F58" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G58" s="2" t="n">
+      <c r="F58" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B59" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C59" s="5" t="s">
+      <c r="C59" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D59" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E59" s="5" t="s">
+      <c r="D59" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E59" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F59" s="5" t="n">
+      <c r="F59" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G59" s="2" t="n">
+      <c r="G59" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B60" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D60" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E60" s="5" t="s">
+      <c r="D60" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E60" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F60" s="5" t="n">
+      <c r="F60" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G60" s="2" t="n">
+      <c r="G60" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B61" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D61" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E61" s="5" t="s">
+      <c r="D61" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E61" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F61" s="5" t="n">
+      <c r="F61" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G61" s="2" t="n">
+      <c r="G61" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B62" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D62" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E62" s="5" t="s">
+      <c r="D62" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F62" s="5" t="n">
+      <c r="F62" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G62" s="2" t="n">
+      <c r="G62" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="5" t="s">
+      <c r="A63" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B63" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D63" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E63" s="5" t="s">
+      <c r="D63" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E63" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="5" t="n">
-        <v>1</v>
-      </c>
-      <c r="G63" s="2" t="n">
+      <c r="F63" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B64" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C64" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D64" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E64" s="5" t="s">
+      <c r="D64" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E64" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F64" s="5" t="n">
+      <c r="F64" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G64" s="2" t="n">
+      <c r="G64" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="5" t="s">
+      <c r="A65" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B65" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D65" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E65" s="5" t="s">
+      <c r="D65" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E65" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F65" s="5" t="n">
+      <c r="F65" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G65" s="2" t="n">
+      <c r="G65" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B66" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D66" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E66" s="5" t="s">
+      <c r="D66" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E66" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F66" s="5" t="n">
+      <c r="F66" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G66" s="2" t="n">
+      <c r="G66" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B67" s="1" t="n">
         <v>10003</v>
       </c>
-      <c r="C67" s="5" t="s">
+      <c r="C67" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D67" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E67" s="5" t="s">
+      <c r="D67" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E67" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F67" s="5" t="n">
+      <c r="F67" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G67" s="2" t="n">
+      <c r="G67" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
[MOSIP-14369] Fix: boolean values
</commit_message>
<xml_diff>
--- a/deployment/v3/mosip/kernel/masterdata/upload/xlsx/app_authentication_method.xlsx
+++ b/deployment/v3/mosip/kernel/masterdata/upload/xlsx/app_authentication_method.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="23">
   <si>
     <t xml:space="preserve">lang_code</t>
   </si>
@@ -55,7 +55,13 @@
     <t xml:space="preserve">PWD</t>
   </si>
   <si>
+    <t xml:space="preserve">TRUE</t>
+  </si>
+  <si>
     <t xml:space="preserve">OTP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FALSE</t>
   </si>
   <si>
     <t xml:space="preserve">FINGERPRINT</t>
@@ -93,7 +99,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -122,6 +128,12 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -173,7 +185,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -191,6 +203,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -214,13 +234,13 @@
   <dimension ref="A1:G67"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H8" activeCellId="0" sqref="H8"/>
+      <selection pane="topLeft" activeCell="J62" activeCellId="0" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.49"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.49"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -265,9 +285,8 @@
       <c r="F2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -284,14 +303,13 @@
         <v>9</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F3" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G3" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -308,14 +326,13 @@
         <v>9</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F4" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G4" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G4" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -332,14 +349,13 @@
         <v>9</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F5" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G5" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G5" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -356,14 +372,13 @@
         <v>9</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F6" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G6" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G6" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -377,7 +392,7 @@
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>10</v>
@@ -385,9 +400,8 @@
       <c r="F7" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G7" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -401,17 +415,16 @@
         <v>8</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F8" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G8" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -425,17 +438,16 @@
         <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F9" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G9" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G9" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -449,17 +461,16 @@
         <v>8</v>
       </c>
       <c r="D10" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="F10" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G10" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G10" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -473,17 +484,16 @@
         <v>8</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F11" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G11" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G11" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>10</v>
@@ -505,9 +515,8 @@
       <c r="F12" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G12" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G12" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -521,17 +530,16 @@
         <v>8</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F13" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G13" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G13" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -545,17 +553,16 @@
         <v>8</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F14" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G14" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G14" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -569,17 +576,16 @@
         <v>8</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F15" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G15" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G15" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -593,17 +599,16 @@
         <v>8</v>
       </c>
       <c r="D16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="F16" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G16" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G16" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -614,7 +619,7 @@
         <v>10003</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D17" s="4" t="s">
         <v>9</v>
@@ -625,9 +630,8 @@
       <c r="F17" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G17" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G17" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -638,20 +642,19 @@
         <v>10003</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F18" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G18" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G18" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -662,10 +665,10 @@
         <v>10003</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E19" s="4" t="s">
         <v>10</v>
@@ -673,9 +676,8 @@
       <c r="F19" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G19" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G19" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,20 +688,19 @@
         <v>10003</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F20" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G20" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G20" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -710,10 +711,10 @@
         <v>10003</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E21" s="4" t="s">
         <v>10</v>
@@ -721,9 +722,8 @@
       <c r="F21" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G21" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -734,20 +734,19 @@
         <v>10003</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F22" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G22" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G22" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -758,7 +757,7 @@
         <v>10003</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D23" s="4" t="s">
         <v>9</v>
@@ -769,9 +768,8 @@
       <c r="F23" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G23" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G23" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -782,20 +780,19 @@
         <v>10003</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F24" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G24" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G24" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -806,20 +803,19 @@
         <v>10003</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F25" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G25" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G25" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -830,20 +826,19 @@
         <v>10003</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F26" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G26" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G26" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -854,20 +849,19 @@
         <v>10003</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F27" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G27" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G27" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -878,10 +872,10 @@
         <v>10003</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>10</v>
@@ -889,9 +883,8 @@
       <c r="F28" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G28" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G28" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -902,20 +895,19 @@
         <v>10003</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F29" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G29" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G29" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -926,20 +918,19 @@
         <v>10003</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F30" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G30" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G30" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,20 +941,19 @@
         <v>10003</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F31" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G31" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G31" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -974,20 +964,19 @@
         <v>10003</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D32" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="F32" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G32" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G32" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -998,10 +987,10 @@
         <v>10003</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>10</v>
@@ -1009,9 +998,8 @@
       <c r="F33" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G33" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G33" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1022,20 +1010,19 @@
         <v>10003</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F34" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G34" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G34" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1046,20 +1033,19 @@
         <v>10003</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F35" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G35" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G35" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1070,20 +1056,19 @@
         <v>10003</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D36" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E36" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="F36" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G36" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G36" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,20 +1079,19 @@
         <v>10003</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F37" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G37" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G37" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1118,7 +1102,7 @@
         <v>10003</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D38" s="4" t="s">
         <v>9</v>
@@ -1129,9 +1113,8 @@
       <c r="F38" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G38" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G38" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,20 +1125,19 @@
         <v>10003</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F39" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G39" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G39" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1166,20 +1148,19 @@
         <v>10003</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F40" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G40" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G40" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1190,20 +1171,19 @@
         <v>10003</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F41" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G41" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G41" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1214,20 +1194,19 @@
         <v>10003</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F42" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G42" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G42" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1238,10 +1217,10 @@
         <v>10003</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>10</v>
@@ -1249,9 +1228,8 @@
       <c r="F43" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G43" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G43" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1262,20 +1240,19 @@
         <v>10003</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F44" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G44" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G44" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1286,20 +1263,19 @@
         <v>10003</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F45" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G45" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G45" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1310,20 +1286,19 @@
         <v>10003</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F46" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G46" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G46" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1334,20 +1309,19 @@
         <v>10003</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D47" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="F47" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G47" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G47" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1358,10 +1332,10 @@
         <v>10003</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>10</v>
@@ -1369,9 +1343,8 @@
       <c r="F48" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G48" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G48" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1382,20 +1355,19 @@
         <v>10003</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F49" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G49" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G49" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1406,20 +1378,19 @@
         <v>10003</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F50" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G50" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G50" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,20 +1401,19 @@
         <v>10003</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D51" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E51" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="F51" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G51" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G51" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1454,20 +1424,19 @@
         <v>10003</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F52" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G52" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G52" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1478,7 +1447,7 @@
         <v>10003</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>9</v>
@@ -1489,9 +1458,8 @@
       <c r="F53" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G53" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G53" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1502,20 +1470,19 @@
         <v>10003</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F54" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G54" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G54" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1526,20 +1493,19 @@
         <v>10003</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F55" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G55" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G55" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1550,20 +1516,19 @@
         <v>10003</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F56" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G56" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G56" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1574,20 +1539,19 @@
         <v>10003</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F57" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G57" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G57" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1598,10 +1562,10 @@
         <v>10003</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E58" s="4" t="s">
         <v>10</v>
@@ -1609,9 +1573,8 @@
       <c r="F58" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G58" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G58" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1622,20 +1585,19 @@
         <v>10003</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F59" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G59" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G59" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1646,20 +1608,19 @@
         <v>10003</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F60" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G60" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G60" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1670,20 +1631,19 @@
         <v>10003</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F61" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G61" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G61" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1694,20 +1654,19 @@
         <v>10003</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D62" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>14</v>
       </c>
       <c r="F62" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G62" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G62" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1718,10 +1677,10 @@
         <v>10003</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E63" s="4" t="s">
         <v>10</v>
@@ -1729,9 +1688,8 @@
       <c r="F63" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="G63" s="1" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="G63" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1742,20 +1700,19 @@
         <v>10003</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F64" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="G64" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G64" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1766,20 +1723,19 @@
         <v>10003</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F65" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="G65" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G65" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1790,20 +1746,19 @@
         <v>10003</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D66" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="E66" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="F66" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="G66" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G66" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1814,20 +1769,19 @@
         <v>10003</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F67" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="G67" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="G67" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>